<commit_message>
Fixing even more filtering log errors
</commit_message>
<xml_diff>
--- a/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/2019_FilteringLog_EDI.xlsx
+++ b/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/2019_FilteringLog_EDI.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cecewood/Documents/Virginia Tech/Sed Traps/2019/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cecewood/Documents/GitHub/Reservoirs/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B64C76-9206-4048-A64C-00CD34C16518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C75FE0-EF04-C047-A43E-7B202854FC36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="275">
   <si>
     <t>Initials</t>
   </si>
@@ -857,6 +857,9 @@
   </si>
   <si>
     <t>F_sed_8m_R2_F2_08Jul19</t>
+  </si>
+  <si>
+    <t>B_sed_5m_R2_F2_08Aug19</t>
   </si>
 </sst>
 </file>
@@ -1836,8 +1839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E95524E5-9B15-A149-8F68-1904FFC7B4AB}">
   <dimension ref="A1:K226"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C138" sqref="C138:C145"/>
+    <sheetView tabSelected="1" topLeftCell="A156" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C172" sqref="C172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6382,7 +6385,7 @@
         <v>43686</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>197</v>
+        <v>274</v>
       </c>
       <c r="E172" s="2">
         <v>0.11409999999999999</v>

</xml_diff>

<commit_message>
Fixing 2019 filtering log errors
</commit_message>
<xml_diff>
--- a/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/2019_FilteringLog_EDI.xlsx
+++ b/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/2019_FilteringLog_EDI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cecewood/Documents/GitHub/Reservoirs/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5863C0-907F-C74A-900A-8C8D73786543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36BB907-27F9-9741-A4EA-677D0CD4A25D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="279">
   <si>
     <t>Initials</t>
   </si>
@@ -860,6 +860,18 @@
   </si>
   <si>
     <t>B_sed_5m_R2_F2_08Aug19</t>
+  </si>
+  <si>
+    <t>F_sed_4m_R2_F2_02Sep19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B_sed_10m_R2_F1_29Apr19 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">B_sed_10m_R2_F2_29Apr19 </t>
+  </si>
+  <si>
+    <t>originally recorded as R1</t>
   </si>
 </sst>
 </file>
@@ -1467,7 +1479,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -1482,6 +1494,7 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1839,8 +1852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E95524E5-9B15-A149-8F68-1904FFC7B4AB}">
   <dimension ref="A1:K226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A156" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C172" sqref="C172"/>
+    <sheetView tabSelected="1" topLeftCell="C107" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K121" sqref="K121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3740,9 +3753,7 @@
       <c r="G74" s="2">
         <v>100</v>
       </c>
-      <c r="H74" s="2">
-        <v>360</v>
-      </c>
+      <c r="H74" s="14"/>
       <c r="I74" s="2"/>
       <c r="J74" s="2">
         <v>14</v>
@@ -3756,7 +3767,7 @@
       <c r="B75" s="3">
         <v>43710</v>
       </c>
-      <c r="C75" s="13" t="s">
+      <c r="C75" s="14" t="s">
         <v>253</v>
       </c>
       <c r="E75" s="2">
@@ -3768,9 +3779,7 @@
       <c r="G75" s="2">
         <v>100</v>
       </c>
-      <c r="H75" s="2">
-        <v>360</v>
-      </c>
+      <c r="H75" s="14"/>
       <c r="I75" s="2"/>
       <c r="J75" s="2">
         <v>14</v>
@@ -3796,9 +3805,7 @@
       <c r="G76" s="2">
         <v>100</v>
       </c>
-      <c r="H76" s="2">
-        <v>370</v>
-      </c>
+      <c r="H76" s="14"/>
       <c r="I76" s="2"/>
       <c r="J76" s="2">
         <v>14</v>
@@ -3812,8 +3819,8 @@
       <c r="B77" s="3">
         <v>43710</v>
       </c>
-      <c r="C77" s="13" t="s">
-        <v>253</v>
+      <c r="C77" s="14" t="s">
+        <v>275</v>
       </c>
       <c r="E77" s="2">
         <v>0.1142</v>
@@ -3824,7 +3831,7 @@
       <c r="G77" s="2">
         <v>100</v>
       </c>
-      <c r="H77" s="2"/>
+      <c r="H77" s="14"/>
       <c r="I77" s="2"/>
       <c r="J77" s="2">
         <v>14</v>
@@ -3848,9 +3855,7 @@
       <c r="G78" s="2">
         <v>100</v>
       </c>
-      <c r="H78" s="13">
-        <v>388</v>
-      </c>
+      <c r="H78" s="14"/>
       <c r="I78" s="2"/>
       <c r="J78" s="2">
         <v>14</v>
@@ -3874,9 +3879,7 @@
       <c r="G79" s="2">
         <v>100</v>
       </c>
-      <c r="H79" s="13">
-        <v>388</v>
-      </c>
+      <c r="H79" s="14"/>
       <c r="I79" s="2"/>
       <c r="J79" s="2">
         <v>14</v>
@@ -3900,9 +3903,7 @@
       <c r="G80" s="2">
         <v>100</v>
       </c>
-      <c r="H80" s="13">
-        <v>365</v>
-      </c>
+      <c r="H80" s="14"/>
       <c r="I80" s="2"/>
       <c r="J80" s="2">
         <v>14</v>
@@ -3926,9 +3927,7 @@
       <c r="G81" s="2">
         <v>100</v>
       </c>
-      <c r="H81" s="13">
-        <v>365</v>
-      </c>
+      <c r="H81" s="14"/>
       <c r="I81" s="2"/>
       <c r="J81" s="2">
         <v>14</v>
@@ -4962,7 +4961,7 @@
       <c r="B118" s="3">
         <v>43585</v>
       </c>
-      <c r="C118" s="13" t="s">
+      <c r="C118" s="14" t="s">
         <v>148</v>
       </c>
       <c r="E118" s="2">
@@ -5014,8 +5013,8 @@
       <c r="B120" s="3">
         <v>43585</v>
       </c>
-      <c r="C120" s="13" t="s">
-        <v>148</v>
+      <c r="C120" s="14" t="s">
+        <v>276</v>
       </c>
       <c r="E120" s="2">
         <v>0.1149</v>
@@ -5031,7 +5030,9 @@
       <c r="J120" s="2">
         <v>21</v>
       </c>
-      <c r="K120" s="2"/>
+      <c r="K120" s="2" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
@@ -5041,7 +5042,7 @@
         <v>43585</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>149</v>
+        <v>277</v>
       </c>
       <c r="E121" s="2">
         <v>0.1147</v>
@@ -5057,7 +5058,9 @@
       <c r="J121" s="2">
         <v>21</v>
       </c>
-      <c r="K121" s="2"/>
+      <c r="K121" s="2" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
@@ -6628,9 +6631,7 @@
       <c r="G181" s="2">
         <v>100</v>
       </c>
-      <c r="H181" s="13">
-        <v>275</v>
-      </c>
+      <c r="H181" s="14"/>
       <c r="I181" s="2"/>
       <c r="J181" s="2">
         <v>14</v>
@@ -6656,9 +6657,7 @@
       <c r="G182" s="2">
         <v>100</v>
       </c>
-      <c r="H182" s="13">
-        <v>275</v>
-      </c>
+      <c r="H182" s="14"/>
       <c r="I182" s="2"/>
       <c r="J182" s="2">
         <v>14</v>
@@ -6684,9 +6683,7 @@
       <c r="G183" s="2">
         <v>100</v>
       </c>
-      <c r="H183" s="13">
-        <v>325</v>
-      </c>
+      <c r="H183" s="14"/>
       <c r="I183" s="2"/>
       <c r="J183" s="2">
         <v>14</v>
@@ -6712,9 +6709,7 @@
       <c r="G184" s="2">
         <v>100</v>
       </c>
-      <c r="H184" s="13">
-        <v>325</v>
-      </c>
+      <c r="H184" s="14"/>
       <c r="I184" s="2"/>
       <c r="J184" s="2">
         <v>14</v>
@@ -6740,9 +6735,7 @@
       <c r="G185" s="2">
         <v>100</v>
       </c>
-      <c r="H185" s="13">
-        <v>335</v>
-      </c>
+      <c r="H185" s="14"/>
       <c r="I185" s="2"/>
       <c r="J185" s="2">
         <v>14</v>
@@ -6768,9 +6761,7 @@
       <c r="G186" s="2">
         <v>100</v>
       </c>
-      <c r="H186" s="13">
-        <v>335</v>
-      </c>
+      <c r="H186" s="14"/>
       <c r="I186" s="2"/>
       <c r="J186" s="2">
         <v>14</v>
@@ -6796,9 +6787,7 @@
       <c r="G187" s="2">
         <v>100</v>
       </c>
-      <c r="H187" s="13">
-        <v>330</v>
-      </c>
+      <c r="H187" s="14"/>
       <c r="I187" s="2"/>
       <c r="J187" s="2">
         <v>13</v>
@@ -6824,9 +6813,7 @@
       <c r="G188" s="2">
         <v>100</v>
       </c>
-      <c r="H188" s="13">
-        <v>330</v>
-      </c>
+      <c r="H188" s="14"/>
       <c r="I188" s="2"/>
       <c r="J188" s="2">
         <v>13</v>
@@ -6852,9 +6839,7 @@
       <c r="G189" s="2">
         <v>100</v>
       </c>
-      <c r="H189" s="13">
-        <v>325</v>
-      </c>
+      <c r="H189" s="14"/>
       <c r="I189" s="2"/>
       <c r="J189" s="2">
         <v>13</v>
@@ -6880,9 +6865,7 @@
       <c r="G190" s="2">
         <v>100</v>
       </c>
-      <c r="H190" s="13">
-        <v>325</v>
-      </c>
+      <c r="H190" s="14"/>
       <c r="I190" s="2"/>
       <c r="J190" s="2">
         <v>13</v>
@@ -6908,9 +6891,7 @@
       <c r="G191" s="2">
         <v>100</v>
       </c>
-      <c r="H191" s="13">
-        <v>325</v>
-      </c>
+      <c r="H191" s="14"/>
       <c r="I191" s="2"/>
       <c r="J191" s="2">
         <v>13</v>
@@ -6936,9 +6917,7 @@
       <c r="G192" s="2">
         <v>100</v>
       </c>
-      <c r="H192" s="13">
-        <v>325</v>
-      </c>
+      <c r="H192" s="14"/>
       <c r="I192" s="2"/>
       <c r="J192" s="2">
         <v>13</v>
@@ -6964,9 +6943,7 @@
       <c r="G193" s="2">
         <v>100</v>
       </c>
-      <c r="H193" s="13">
-        <v>350</v>
-      </c>
+      <c r="H193" s="14"/>
       <c r="I193" s="2"/>
       <c r="J193" s="2">
         <v>13</v>
@@ -6992,9 +6969,7 @@
       <c r="G194" s="2">
         <v>100</v>
       </c>
-      <c r="H194" s="13">
-        <v>350</v>
-      </c>
+      <c r="H194" s="14"/>
       <c r="I194" s="2"/>
       <c r="J194" s="2">
         <v>13</v>

</xml_diff>